<commit_message>
add tool based fixes
</commit_message>
<xml_diff>
--- a/Docs/Lab1/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab1/Lab01_ReviewReport.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Facultate\An3Sem2\vvss\Docs\Lab1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61031373-1545-4359-A49A-9D7FC1CE23C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="650" activeTab="1"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -12,12 +18,12 @@
     <sheet name="Coding Phase Defects" sheetId="5" r:id="rId3"/>
     <sheet name="Tool-basedCodeAnalysis" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="70">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -191,13 +197,49 @@
   </si>
   <si>
     <t>Clasa MainGuiController nu reflecta faptul ca este un meniu pentru mese</t>
+  </si>
+  <si>
+    <t>KitchenGUI</t>
+  </si>
+  <si>
+    <t>The name of the function can be confused for a constructor</t>
+  </si>
+  <si>
+    <t>initKitchenGUI</t>
+  </si>
+  <si>
+    <t>KitchenGUI/28</t>
+  </si>
+  <si>
+    <t>OrdersGUIController/55</t>
+  </si>
+  <si>
+    <t>Instance methods should not write to "static" fields</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        this.totalAmount = totalAmount;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        OrdersGUIController.totalAmount = totalAmount; and made the function static</t>
+  </si>
+  <si>
+    <t>Sections of code should not be commented out</t>
+  </si>
+  <si>
+    <t>OrdersGUIController/63</t>
+  </si>
+  <si>
+    <t>// = FXCollections.observableArrayList();</t>
+  </si>
+  <si>
+    <t>deleted the comment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -416,10 +458,16 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -428,14 +476,20 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -451,18 +505,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -524,7 +566,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -556,9 +598,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -590,6 +650,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -765,7 +843,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
@@ -775,7 +853,7 @@
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="6"/>
     <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
@@ -787,32 +865,32 @@
     <col min="11" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="40" t="s">
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="39"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="27"/>
       <c r="B2" s="22" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
       <c r="H2" s="20"/>
       <c r="I2" s="20" t="s">
         <v>29</v>
@@ -821,14 +899,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="39"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
       <c r="H3" s="20" t="s">
         <v>19</v>
       </c>
@@ -839,9 +917,9 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="39"/>
-      <c r="B4" s="39"/>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
       <c r="C4" s="14" t="s">
         <v>0</v>
       </c>
@@ -849,8 +927,8 @@
         <v>13</v>
       </c>
       <c r="E4" s="23"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
       <c r="H4" s="20" t="s">
         <v>20</v>
       </c>
@@ -861,9 +939,9 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="39"/>
-      <c r="B5" s="39"/>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
       <c r="C5" s="14" t="s">
         <v>9</v>
       </c>
@@ -871,16 +949,16 @@
         <v>12</v>
       </c>
       <c r="E5" s="25"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
       <c r="H5" s="20" t="s">
         <v>21</v>
       </c>
       <c r="I5" s="20"/>
       <c r="J5" s="20"/>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="39"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="27"/>
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
@@ -889,15 +967,15 @@
         <v>41</v>
       </c>
       <c r="E6" s="21"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="39"/>
-      <c r="B7" s="39"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
@@ -905,26 +983,26 @@
         <v>44262</v>
       </c>
       <c r="E7" s="21"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="39"/>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="39"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="27"/>
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -937,14 +1015,14 @@
       <c r="E9" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="39"/>
-    </row>
-    <row r="10" spans="1:10" ht="45">
-      <c r="A10" s="39"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+    </row>
+    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="27"/>
       <c r="B10" s="20">
         <v>1</v>
       </c>
@@ -957,14 +1035,14 @@
       <c r="E10" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="39"/>
-    </row>
-    <row r="11" spans="1:10" ht="30">
-      <c r="A11" s="39"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+    </row>
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="27"/>
       <c r="B11" s="20">
         <v>2</v>
       </c>
@@ -977,14 +1055,14 @@
       <c r="E11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="39"/>
-    </row>
-    <row r="12" spans="1:10" ht="30">
-      <c r="A12" s="39"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+    </row>
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="27"/>
       <c r="B12" s="20">
         <v>3</v>
       </c>
@@ -995,14 +1073,14 @@
       <c r="E12" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="39"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="27"/>
       <c r="B13" s="20">
         <v>4</v>
       </c>
@@ -1011,195 +1089,195 @@
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="39"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="39"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="27"/>
       <c r="B14" s="20">
         <v>5</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="D14" s="41"/>
+      <c r="D14" s="29"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="39"/>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="39"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="27"/>
       <c r="B15" s="20">
         <v>6</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="39"/>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="39"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="27"/>
       <c r="B16" s="20">
         <v>7</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="39"/>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="39"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="27"/>
       <c r="B17" s="20">
         <v>8</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="39"/>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="39"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="27"/>
       <c r="B18" s="20">
         <v>9</v>
       </c>
       <c r="C18" s="20"/>
       <c r="D18" s="20"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="39"/>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="39"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="27"/>
       <c r="B19" s="20">
         <v>10</v>
       </c>
       <c r="C19" s="20"/>
       <c r="D19" s="20"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="39"/>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="39"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="27"/>
       <c r="B20" s="20">
         <v>11</v>
       </c>
       <c r="C20" s="20"/>
       <c r="D20" s="20"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="39"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="27"/>
       <c r="B21" s="20">
         <v>12</v>
       </c>
       <c r="C21" s="20"/>
       <c r="D21" s="20"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="39"/>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="39"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="27"/>
       <c r="B22" s="20">
         <v>13</v>
       </c>
       <c r="C22" s="20"/>
       <c r="D22" s="20"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="39"/>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="39"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="27"/>
       <c r="B23" s="20">
         <v>14</v>
       </c>
       <c r="C23" s="20"/>
       <c r="D23" s="20"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="39"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="27"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="27"/>
       <c r="B24" s="20">
         <v>15</v>
       </c>
       <c r="C24" s="20"/>
       <c r="D24" s="20"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="39"/>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="39"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="27"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="27"/>
       <c r="B25" s="20">
         <v>16</v>
       </c>
       <c r="C25" s="20"/>
       <c r="D25" s="20"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
-      <c r="I25" s="39"/>
-      <c r="J25" s="39"/>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="39"/>
-      <c r="B26" s="39"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="39"/>
-      <c r="J26" s="39"/>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="39"/>
-      <c r="B27" s="39"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="27"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="27"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="27"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="27"/>
+      <c r="B27" s="27"/>
       <c r="C27" s="12" t="s">
         <v>8</v>
       </c>
@@ -1207,11 +1285,11 @@
       <c r="E27" s="1">
         <v>2</v>
       </c>
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="39"/>
-      <c r="I27" s="39"/>
-      <c r="J27" s="39"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="27"/>
+      <c r="J27" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1220,17 +1298,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="6"/>
     <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
@@ -1241,32 +1319,32 @@
     <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="44" t="s">
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="39"/>
-      <c r="B2" s="29" t="s">
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="27"/>
+      <c r="B2" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
       <c r="H2" s="20"/>
       <c r="I2" s="20" t="s">
         <v>29</v>
@@ -1275,14 +1353,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="39"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
       <c r="H3" s="20" t="s">
         <v>19</v>
       </c>
@@ -1293,18 +1371,18 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="39"/>
-      <c r="B4" s="39"/>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="30"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
       <c r="H4" s="20" t="s">
         <v>20</v>
       </c>
@@ -1315,70 +1393,70 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="39"/>
-      <c r="B5" s="39"/>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="32"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
       <c r="H5" s="20" t="s">
         <v>21</v>
       </c>
       <c r="I5" s="20"/>
       <c r="J5" s="20"/>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="39"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="27"/>
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="27"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="39"/>
-      <c r="B7" s="39"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7" s="36">
         <v>44263</v>
       </c>
-      <c r="E7" s="27"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="39"/>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="39"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="27"/>
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1391,14 +1469,14 @@
       <c r="E9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="39"/>
-    </row>
-    <row r="10" spans="1:10" ht="30">
-      <c r="A10" s="39"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+    </row>
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="27"/>
       <c r="B10" s="20">
         <v>1</v>
       </c>
@@ -1409,14 +1487,14 @@
       <c r="E10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="39"/>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="39"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="27"/>
       <c r="B11" s="20">
         <f>B10+1</f>
         <v>2</v>
@@ -1428,14 +1506,14 @@
       <c r="E11" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="39"/>
-    </row>
-    <row r="12" spans="1:10" ht="30">
-      <c r="A12" s="39"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+    </row>
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="27"/>
       <c r="B12" s="20">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
@@ -1447,14 +1525,14 @@
       <c r="E12" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="39"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="27"/>
       <c r="B13" s="20">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1462,14 +1540,14 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="39"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="39"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="27"/>
       <c r="B14" s="20">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1477,14 +1555,14 @@
       <c r="C14" s="1"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="39"/>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="39"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="27"/>
       <c r="B15" s="20">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1492,14 +1570,14 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="39"/>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="39"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="27"/>
       <c r="B16" s="20">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1507,14 +1585,14 @@
       <c r="C16" s="1"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="39"/>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="39"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="27"/>
       <c r="B17" s="20">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1522,14 +1600,14 @@
       <c r="C17" s="1"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="39"/>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="39"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="27"/>
       <c r="B18" s="20">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1537,14 +1615,14 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="39"/>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="39"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="27"/>
       <c r="B19" s="20">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1552,14 +1630,14 @@
       <c r="C19" s="1"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="39"/>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="39"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="27"/>
       <c r="B20" s="20">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1567,14 +1645,14 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="39"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="27"/>
       <c r="B21" s="20">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1582,14 +1660,14 @@
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="39"/>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="39"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="27"/>
       <c r="B22" s="20">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1597,14 +1675,14 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="39"/>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="39"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="27"/>
       <c r="B23" s="20">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1612,14 +1690,14 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="39"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="27"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="27"/>
       <c r="B24" s="20">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1627,14 +1705,14 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="39"/>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="39"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="27"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="27"/>
       <c r="B25" s="20">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1642,14 +1720,14 @@
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
-      <c r="I25" s="39"/>
-      <c r="J25" s="39"/>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="39"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="27"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="27"/>
       <c r="B26" s="20">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1657,27 +1735,27 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="39"/>
-      <c r="J26" s="39"/>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="39"/>
-      <c r="B27" s="39"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="39"/>
-      <c r="I27" s="39"/>
-      <c r="J27" s="39"/>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="39"/>
-      <c r="B28" s="39"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="27"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="27"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="27"/>
+      <c r="J27" s="27"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="27"/>
+      <c r="B28" s="27"/>
       <c r="C28" s="12" t="s">
         <v>8</v>
       </c>
@@ -1685,11 +1763,11 @@
       <c r="E28" s="1">
         <v>4</v>
       </c>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="39"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1706,7 +1784,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
@@ -1716,7 +1794,7 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="6"/>
     <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
@@ -1728,24 +1806,24 @@
     <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="H1" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="B2" s="29" t="s">
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>29</v>
@@ -1754,61 +1832,61 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="18" t="s">
         <v>19</v>
       </c>
       <c r="I3" s="18"/>
       <c r="J3" s="18"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="34"/>
+      <c r="E4" s="40"/>
       <c r="H4" s="18" t="s">
         <v>20</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="36"/>
+      <c r="E5" s="42"/>
       <c r="H5" s="18" t="s">
         <v>21</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="27"/>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="E6" s="35"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7" s="36">
         <v>44380</v>
       </c>
-      <c r="E7" s="27"/>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="E7" s="35"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>4</v>
       </c>
@@ -1822,7 +1900,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30" customHeight="1">
+    <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="16">
         <v>1</v>
       </c>
@@ -1836,7 +1914,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="45">
+    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="16">
         <f>B10+1</f>
         <v>2</v>
@@ -1851,7 +1929,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="30">
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="16">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -1866,7 +1944,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="16">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1875,7 +1953,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="16">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1884,7 +1962,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="16">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1893,7 +1971,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="16">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1902,7 +1980,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="16">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1911,7 +1989,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="16">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1920,7 +1998,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="16">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1929,7 +2007,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="16">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1938,7 +2016,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="16">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1947,7 +2025,7 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="16">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1956,7 +2034,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="16">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1965,7 +2043,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1974,7 +2052,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="16">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1983,7 +2061,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="16">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1992,7 +2070,7 @@
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="16">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2001,7 +2079,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="2:5">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="16">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2010,7 +2088,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="16">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2019,7 +2097,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="16">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2028,10 +2106,10 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="2:5">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="2:5">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C32" s="12" t="s">
         <v>8</v>
       </c>
@@ -2053,17 +2131,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="6" tint="0.79998168889431442"/>
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="6"/>
     <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
@@ -2076,24 +2154,24 @@
     <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="H1" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="B2" s="29" t="s">
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>29</v>
@@ -2102,281 +2180,307 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="18" t="s">
         <v>19</v>
       </c>
       <c r="I3" s="18"/>
       <c r="J3" s="18"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
       <c r="H4" s="18" t="s">
         <v>20</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
       <c r="H5" s="18" t="s">
         <v>21</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="B9" s="10" t="s">
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
-      <c r="B10" s="3">
+    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="B10" s="16">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="B11" s="3">
+      <c r="C10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="B11" s="16">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="B12" s="3">
+      <c r="C11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B12" s="16">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="B13" s="3">
+      <c r="C12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="16">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:10">
-      <c r="B14" s="3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="16">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
+      <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:10">
-      <c r="B15" s="3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="16">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
+      <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:10">
-      <c r="B16" s="3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="16">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="1"/>
+      <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:6">
-      <c r="B17" s="3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="16">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="1"/>
+      <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6">
-      <c r="B18" s="3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="16">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="1"/>
+      <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6">
-      <c r="B19" s="3">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="16">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6">
-      <c r="B20" s="3">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="16">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C20" s="1"/>
+      <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6">
-      <c r="B21" s="3">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="16">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6">
-      <c r="B22" s="3">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="16">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C22" s="1"/>
+      <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6">
-      <c r="B23" s="3">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="16">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C23" s="1"/>
+      <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6">
-      <c r="B24" s="3">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="16">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C24" s="1"/>
+      <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6">
-      <c r="B25" s="3">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="16">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C25" s="1"/>
+      <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6">
-      <c r="B26" s="3">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="16">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6">
-      <c r="B27" s="3">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="16">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C27" s="1"/>
+      <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="2:6">
-      <c r="B28" s="3">
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="16">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C28" s="1"/>
+      <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6">
-      <c r="B29" s="3">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="16">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C29" s="1"/>
+      <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6">
-      <c r="B30" s="3">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="16">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C30" s="1"/>
+      <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="2:6">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="2:6">
-      <c r="C32" s="37" t="s">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C32" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="D32" s="38"/>
-      <c r="E32" s="38"/>
-      <c r="F32" s="19"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="19">
+        <v>0.5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
am schimbat numele clasei MainGuiController
MainGuiController -> MeseGuiController
</commit_message>
<xml_diff>
--- a/Docs/Lab1/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab1/Lab01_ReviewReport.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Facultate\An3Sem2\vvss\Docs\Lab1\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13A9530-9F41-4E3E-B9A9-D7BD9C1F9434}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -18,12 +12,12 @@
     <sheet name="Coding Phase Defects" sheetId="5" r:id="rId3"/>
     <sheet name="Tool-basedCodeAnalysis" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="77">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -187,12 +181,6 @@
     <t>Partea de requirements cu inchiderea restaurantuli nu este prezenta in model</t>
   </si>
   <si>
-    <t>A05</t>
-  </si>
-  <si>
-    <t>No error handling</t>
-  </si>
-  <si>
     <t>A07</t>
   </si>
   <si>
@@ -257,13 +245,16 @@
   </si>
   <si>
     <t>deleted the import</t>
+  </si>
+  <si>
+    <t>Partea de requirements cu inchiderea bucatariei nu este prezenta in model</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -590,7 +581,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -622,27 +613,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -674,24 +647,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -867,7 +822,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
@@ -877,7 +832,7 @@
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="6"/>
     <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
@@ -889,7 +844,7 @@
     <col min="11" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -905,7 +860,7 @@
       <c r="I1" s="28"/>
       <c r="J1" s="28"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="27"/>
       <c r="B2" s="22" t="s">
         <v>18</v>
@@ -923,7 +878,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="27"/>
       <c r="B3" s="27"/>
       <c r="C3" s="27"/>
@@ -941,7 +896,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="27"/>
       <c r="B4" s="27"/>
       <c r="C4" s="14" t="s">
@@ -963,7 +918,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="27"/>
       <c r="B5" s="27"/>
       <c r="C5" s="14" t="s">
@@ -981,7 +936,7 @@
       <c r="I5" s="20"/>
       <c r="J5" s="20"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="27"/>
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
@@ -997,7 +952,7 @@
       <c r="I6" s="27"/>
       <c r="J6" s="27"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="27"/>
       <c r="B7" s="27"/>
       <c r="C7" s="9" t="s">
@@ -1013,7 +968,7 @@
       <c r="I7" s="27"/>
       <c r="J7" s="27"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="27"/>
       <c r="B8" s="27"/>
       <c r="C8" s="27"/>
@@ -1025,7 +980,7 @@
       <c r="I8" s="27"/>
       <c r="J8" s="27"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="27"/>
       <c r="B9" s="10" t="s">
         <v>4</v>
@@ -1045,7 +1000,7 @@
       <c r="I9" s="27"/>
       <c r="J9" s="27"/>
     </row>
-    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="45">
       <c r="A10" s="27"/>
       <c r="B10" s="20">
         <v>1</v>
@@ -1065,7 +1020,7 @@
       <c r="I10" s="27"/>
       <c r="J10" s="27"/>
     </row>
-    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="30">
       <c r="A11" s="27"/>
       <c r="B11" s="20">
         <v>2</v>
@@ -1085,7 +1040,7 @@
       <c r="I11" s="27"/>
       <c r="J11" s="27"/>
     </row>
-    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="30">
       <c r="A12" s="27"/>
       <c r="B12" s="20">
         <v>3</v>
@@ -1103,7 +1058,7 @@
       <c r="I12" s="27"/>
       <c r="J12" s="27"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="27"/>
       <c r="B13" s="20">
         <v>4</v>
@@ -1119,7 +1074,7 @@
       <c r="I13" s="27"/>
       <c r="J13" s="27"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="27"/>
       <c r="B14" s="20">
         <v>5</v>
@@ -1133,7 +1088,7 @@
       <c r="I14" s="27"/>
       <c r="J14" s="27"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="27"/>
       <c r="B15" s="20">
         <v>6</v>
@@ -1147,7 +1102,7 @@
       <c r="I15" s="27"/>
       <c r="J15" s="27"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="27"/>
       <c r="B16" s="20">
         <v>7</v>
@@ -1161,7 +1116,7 @@
       <c r="I16" s="27"/>
       <c r="J16" s="27"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="27"/>
       <c r="B17" s="20">
         <v>8</v>
@@ -1175,7 +1130,7 @@
       <c r="I17" s="27"/>
       <c r="J17" s="27"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="27"/>
       <c r="B18" s="20">
         <v>9</v>
@@ -1189,7 +1144,7 @@
       <c r="I18" s="27"/>
       <c r="J18" s="27"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="27"/>
       <c r="B19" s="20">
         <v>10</v>
@@ -1203,7 +1158,7 @@
       <c r="I19" s="27"/>
       <c r="J19" s="27"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="27"/>
       <c r="B20" s="20">
         <v>11</v>
@@ -1217,7 +1172,7 @@
       <c r="I20" s="27"/>
       <c r="J20" s="27"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="27"/>
       <c r="B21" s="20">
         <v>12</v>
@@ -1231,7 +1186,7 @@
       <c r="I21" s="27"/>
       <c r="J21" s="27"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="27"/>
       <c r="B22" s="20">
         <v>13</v>
@@ -1245,7 +1200,7 @@
       <c r="I22" s="27"/>
       <c r="J22" s="27"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="27"/>
       <c r="B23" s="20">
         <v>14</v>
@@ -1259,7 +1214,7 @@
       <c r="I23" s="27"/>
       <c r="J23" s="27"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="27"/>
       <c r="B24" s="20">
         <v>15</v>
@@ -1273,7 +1228,7 @@
       <c r="I24" s="27"/>
       <c r="J24" s="27"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="27"/>
       <c r="B25" s="20">
         <v>16</v>
@@ -1287,7 +1242,7 @@
       <c r="I25" s="27"/>
       <c r="J25" s="27"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="27"/>
       <c r="B26" s="27"/>
       <c r="C26" s="27"/>
@@ -1299,7 +1254,7 @@
       <c r="I26" s="27"/>
       <c r="J26" s="27"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="27"/>
       <c r="B27" s="27"/>
       <c r="C27" s="12" t="s">
@@ -1322,17 +1277,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="6"/>
     <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
@@ -1343,7 +1298,7 @@
     <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -1359,7 +1314,7 @@
       <c r="I1" s="32"/>
       <c r="J1" s="32"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="27"/>
       <c r="B2" s="33" t="s">
         <v>17</v>
@@ -1377,7 +1332,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="27"/>
       <c r="B3" s="27"/>
       <c r="C3" s="27"/>
@@ -1395,7 +1350,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="27"/>
       <c r="B4" s="27"/>
       <c r="C4" s="7" t="s">
@@ -1417,7 +1372,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="27"/>
       <c r="B5" s="27"/>
       <c r="C5" s="7" t="s">
@@ -1435,7 +1390,7 @@
       <c r="I5" s="20"/>
       <c r="J5" s="20"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="27"/>
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
@@ -1451,7 +1406,7 @@
       <c r="I6" s="27"/>
       <c r="J6" s="27"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="27"/>
       <c r="B7" s="27"/>
       <c r="C7" s="9" t="s">
@@ -1467,7 +1422,7 @@
       <c r="I7" s="27"/>
       <c r="J7" s="27"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="27"/>
       <c r="B8" s="27"/>
       <c r="C8" s="27"/>
@@ -1479,7 +1434,7 @@
       <c r="I8" s="27"/>
       <c r="J8" s="27"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="27"/>
       <c r="B9" s="10" t="s">
         <v>4</v>
@@ -1499,7 +1454,7 @@
       <c r="I9" s="27"/>
       <c r="J9" s="27"/>
     </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="30">
       <c r="A10" s="27"/>
       <c r="B10" s="20">
         <v>1</v>
@@ -1517,18 +1472,18 @@
       <c r="I10" s="27"/>
       <c r="J10" s="27"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="30">
       <c r="A11" s="27"/>
       <c r="B11" s="20">
         <f>B10+1</f>
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="F11" s="27"/>
       <c r="G11" s="27"/>
@@ -1536,18 +1491,18 @@
       <c r="I11" s="27"/>
       <c r="J11" s="27"/>
     </row>
-    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="30">
       <c r="A12" s="27"/>
       <c r="B12" s="20">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F12" s="27"/>
       <c r="G12" s="27"/>
@@ -1555,7 +1510,7 @@
       <c r="I12" s="27"/>
       <c r="J12" s="27"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="27"/>
       <c r="B13" s="20">
         <f t="shared" si="0"/>
@@ -1570,7 +1525,7 @@
       <c r="I13" s="27"/>
       <c r="J13" s="27"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="27"/>
       <c r="B14" s="20">
         <f t="shared" si="0"/>
@@ -1585,7 +1540,7 @@
       <c r="I14" s="27"/>
       <c r="J14" s="27"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="27"/>
       <c r="B15" s="20">
         <f t="shared" si="0"/>
@@ -1600,7 +1555,7 @@
       <c r="I15" s="27"/>
       <c r="J15" s="27"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="27"/>
       <c r="B16" s="20">
         <f t="shared" si="0"/>
@@ -1615,7 +1570,7 @@
       <c r="I16" s="27"/>
       <c r="J16" s="27"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="27"/>
       <c r="B17" s="20">
         <f t="shared" si="0"/>
@@ -1630,7 +1585,7 @@
       <c r="I17" s="27"/>
       <c r="J17" s="27"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="27"/>
       <c r="B18" s="20">
         <f t="shared" si="0"/>
@@ -1645,7 +1600,7 @@
       <c r="I18" s="27"/>
       <c r="J18" s="27"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="27"/>
       <c r="B19" s="20">
         <f t="shared" si="0"/>
@@ -1660,7 +1615,7 @@
       <c r="I19" s="27"/>
       <c r="J19" s="27"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="27"/>
       <c r="B20" s="20">
         <f t="shared" si="0"/>
@@ -1675,7 +1630,7 @@
       <c r="I20" s="27"/>
       <c r="J20" s="27"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="27"/>
       <c r="B21" s="20">
         <f t="shared" si="0"/>
@@ -1690,7 +1645,7 @@
       <c r="I21" s="27"/>
       <c r="J21" s="27"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="27"/>
       <c r="B22" s="20">
         <f t="shared" si="0"/>
@@ -1705,7 +1660,7 @@
       <c r="I22" s="27"/>
       <c r="J22" s="27"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="27"/>
       <c r="B23" s="20">
         <f t="shared" si="0"/>
@@ -1720,7 +1675,7 @@
       <c r="I23" s="27"/>
       <c r="J23" s="27"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="27"/>
       <c r="B24" s="20">
         <f t="shared" si="0"/>
@@ -1735,7 +1690,7 @@
       <c r="I24" s="27"/>
       <c r="J24" s="27"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="27"/>
       <c r="B25" s="20">
         <f t="shared" si="0"/>
@@ -1750,7 +1705,7 @@
       <c r="I25" s="27"/>
       <c r="J25" s="27"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="27"/>
       <c r="B26" s="20">
         <f t="shared" si="0"/>
@@ -1765,7 +1720,7 @@
       <c r="I26" s="27"/>
       <c r="J26" s="27"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="27"/>
       <c r="B27" s="27"/>
       <c r="C27" s="27"/>
@@ -1777,7 +1732,7 @@
       <c r="I27" s="27"/>
       <c r="J27" s="27"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="27"/>
       <c r="B28" s="27"/>
       <c r="C28" s="12" t="s">
@@ -1808,7 +1763,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
@@ -1818,7 +1773,7 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="6"/>
     <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
@@ -1830,7 +1785,7 @@
     <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -1841,7 +1796,7 @@
       <c r="I1" s="39"/>
       <c r="J1" s="39"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="B2" s="33" t="s">
         <v>16</v>
       </c>
@@ -1856,14 +1811,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="H3" s="18" t="s">
         <v>19</v>
       </c>
       <c r="I3" s="18"/>
       <c r="J3" s="18"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="C4" s="17" t="s">
         <v>0</v>
       </c>
@@ -1877,7 +1832,7 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="C5" s="17" t="s">
         <v>9</v>
       </c>
@@ -1891,7 +1846,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
@@ -1901,7 +1856,7 @@
       </c>
       <c r="E6" s="35"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
@@ -1910,7 +1865,7 @@
       </c>
       <c r="E7" s="35"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="B9" s="15" t="s">
         <v>4</v>
       </c>
@@ -1924,7 +1879,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="30" customHeight="1">
       <c r="B10" s="16">
         <v>1</v>
       </c>
@@ -1938,7 +1893,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="45">
       <c r="B11" s="16">
         <f>B10+1</f>
         <v>2</v>
@@ -1953,7 +1908,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="30">
       <c r="B12" s="16">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -1968,7 +1923,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="B13" s="16">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1977,7 +1932,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="B14" s="16">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1986,7 +1941,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="B15" s="16">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1995,7 +1950,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="B16" s="16">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2004,7 +1959,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5">
       <c r="B17" s="16">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2013,7 +1968,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5">
       <c r="B18" s="16">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2022,7 +1977,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5">
       <c r="B19" s="16">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2031,7 +1986,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5">
       <c r="B20" s="16">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2040,7 +1995,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5">
       <c r="B21" s="16">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2049,7 +2004,7 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5">
       <c r="B22" s="16">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2058,7 +2013,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5">
       <c r="B23" s="16">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2067,7 +2022,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5">
       <c r="B24" s="16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2076,7 +2031,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5">
       <c r="B25" s="16">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2085,7 +2040,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5">
       <c r="B26" s="16">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2094,7 +2049,7 @@
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5">
       <c r="B27" s="16">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2103,7 +2058,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5">
       <c r="B28" s="16">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2112,7 +2067,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5">
       <c r="B29" s="16">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2121,7 +2076,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5">
       <c r="B30" s="16">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2130,10 +2085,10 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5">
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5">
       <c r="C32" s="12" t="s">
         <v>8</v>
       </c>
@@ -2155,17 +2110,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="6" tint="0.79998168889431442"/>
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="6"/>
     <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
@@ -2178,7 +2133,7 @@
     <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -2189,7 +2144,7 @@
       <c r="I1" s="39"/>
       <c r="J1" s="39"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="B2" s="33" t="s">
         <v>30</v>
       </c>
@@ -2204,14 +2159,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="H3" s="18" t="s">
         <v>19</v>
       </c>
       <c r="I3" s="18"/>
       <c r="J3" s="18"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="C4" s="17" t="s">
         <v>24</v>
       </c>
@@ -2223,7 +2178,7 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
@@ -2235,7 +2190,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>1</v>
@@ -2243,7 +2198,7 @@
       <c r="D6" s="35"/>
       <c r="E6" s="35"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="B9" s="15" t="s">
         <v>4</v>
       </c>
@@ -2260,96 +2215,96 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="60">
       <c r="B10" s="16">
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:10" ht="90">
       <c r="B11" s="16">
         <f>B10+1</f>
         <v>2</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:10" ht="45">
       <c r="B12" s="16">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E12" s="2" t="s">
+    </row>
+    <row r="13" spans="1:10" ht="60">
+      <c r="B13" s="16">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="B13" s="16">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E13" s="2" t="s">
+    </row>
+    <row r="14" spans="1:10" ht="45">
+      <c r="B14" s="16">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B14" s="16">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:10">
       <c r="B15" s="16">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2359,7 +2314,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="B16" s="16">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2369,7 +2324,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6">
       <c r="B17" s="16">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2379,7 +2334,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6">
       <c r="B18" s="16">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2389,7 +2344,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6">
       <c r="B19" s="16">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2399,7 +2354,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6">
       <c r="B20" s="16">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2409,7 +2364,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6">
       <c r="B21" s="16">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2419,7 +2374,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6">
       <c r="B22" s="16">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2429,7 +2384,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6">
       <c r="B23" s="16">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2439,7 +2394,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6">
       <c r="B24" s="16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2449,7 +2404,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6">
       <c r="B25" s="16">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2459,7 +2414,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6">
       <c r="B26" s="16">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2469,7 +2424,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6">
       <c r="B27" s="16">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2479,7 +2434,7 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6">
       <c r="B28" s="16">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2489,7 +2444,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6">
       <c r="B29" s="16">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2499,7 +2454,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6">
       <c r="B30" s="16">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2509,10 +2464,10 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6">
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6">
       <c r="C32" s="43" t="s">
         <v>31</v>
       </c>

</xml_diff>